<commit_message>
Fix header handling in Excel table creation to support merged cells
Co-authored-by: borgesr18 <borgesr18@yahoo.com.br>
</commit_message>
<xml_diff>
--- a/Planilha SOSrim (Melhorada).xlsx
+++ b/Planilha SOSrim (Melhorada).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PLANILHA ATRAS. JAN. A JUL 2025" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PLANILHA ACORDO " sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PLANILHA PAGTOS JULHO 2025" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PLANILHA PAGTOS ACORDOS FORN." sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dashboard_Auto" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="PLANILHA ATRAS. JAN. A JUL 2025" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="PLANILHA ACORDO " sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="PLANILHA PAGTOS JULHO 2025" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="PLANILHA PAGTOS ACORDOS FORN." sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Dashboard_Auto" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PLANILHA ATRAS. JAN. A JUL 2025'!$A$1:$L$264</definedName>
@@ -2835,13 +2835,13 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -2865,7 +2865,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -2893,8 +2893,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -2920,8 +2920,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -2947,7 +2947,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>4</col>
@@ -2962,9 +2962,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -2978,17 +2978,17 @@
   <autoFilter ref="A1:L264"/>
   <tableColumns count="12">
     <tableColumn id="1" name="CLÍNICA NEFROLÓGICA DE CARUARU LTDA."/>
-    <tableColumn id="2" name="None"/>
-    <tableColumn id="3" name="None"/>
-    <tableColumn id="4" name="None"/>
-    <tableColumn id="5" name="None"/>
-    <tableColumn id="6" name="None"/>
-    <tableColumn id="7" name="None"/>
-    <tableColumn id="8" name="None"/>
-    <tableColumn id="9" name="None"/>
-    <tableColumn id="10" name="None"/>
-    <tableColumn id="11" name="None"/>
-    <tableColumn id="12" name="None"/>
+    <tableColumn id="2" name="Coluna_B"/>
+    <tableColumn id="3" name="Coluna_C"/>
+    <tableColumn id="4" name="Coluna_D"/>
+    <tableColumn id="5" name="Coluna_E"/>
+    <tableColumn id="6" name="Coluna_F"/>
+    <tableColumn id="7" name="Coluna_G"/>
+    <tableColumn id="8" name="Coluna_H"/>
+    <tableColumn id="9" name="Coluna_I"/>
+    <tableColumn id="10" name="Coluna_J"/>
+    <tableColumn id="11" name="Coluna_K"/>
+    <tableColumn id="12" name="Coluna_L"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2998,53 +2998,53 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="PLANILHAACORDOTable" displayName="PLANILHAACORDOTable" ref="B1:AV49" headerRowCount="1">
   <autoFilter ref="B1:AV49"/>
   <tableColumns count="47">
-    <tableColumn id="2" name="None"/>
-    <tableColumn id="3" name="None"/>
-    <tableColumn id="4" name="None"/>
-    <tableColumn id="5" name="None"/>
-    <tableColumn id="6" name="None"/>
-    <tableColumn id="7" name="None"/>
-    <tableColumn id="8" name="None"/>
-    <tableColumn id="9" name="None"/>
-    <tableColumn id="10" name="None"/>
-    <tableColumn id="11" name="None"/>
-    <tableColumn id="12" name="None"/>
-    <tableColumn id="13" name="None"/>
-    <tableColumn id="14" name="None"/>
-    <tableColumn id="15" name="None"/>
-    <tableColumn id="16" name="None"/>
-    <tableColumn id="17" name="None"/>
-    <tableColumn id="18" name="None"/>
-    <tableColumn id="19" name="None"/>
-    <tableColumn id="20" name="None"/>
-    <tableColumn id="21" name="None"/>
-    <tableColumn id="22" name="None"/>
-    <tableColumn id="23" name="None"/>
-    <tableColumn id="24" name="None"/>
-    <tableColumn id="25" name="None"/>
-    <tableColumn id="26" name="None"/>
-    <tableColumn id="27" name="None"/>
-    <tableColumn id="28" name="None"/>
-    <tableColumn id="29" name="None"/>
-    <tableColumn id="30" name="None"/>
-    <tableColumn id="31" name="None"/>
-    <tableColumn id="32" name="None"/>
-    <tableColumn id="33" name="None"/>
-    <tableColumn id="34" name="None"/>
-    <tableColumn id="35" name="None"/>
-    <tableColumn id="36" name="None"/>
-    <tableColumn id="37" name="None"/>
-    <tableColumn id="38" name="None"/>
-    <tableColumn id="39" name="None"/>
-    <tableColumn id="40" name="None"/>
-    <tableColumn id="41" name="None"/>
-    <tableColumn id="42" name="None"/>
-    <tableColumn id="43" name="None"/>
-    <tableColumn id="44" name="None"/>
-    <tableColumn id="45" name="None"/>
-    <tableColumn id="46" name="None"/>
-    <tableColumn id="47" name="None"/>
-    <tableColumn id="48" name="None"/>
+    <tableColumn id="2" name="Coluna_B"/>
+    <tableColumn id="3" name="Coluna_C"/>
+    <tableColumn id="4" name="Coluna_D"/>
+    <tableColumn id="5" name="Coluna_E"/>
+    <tableColumn id="6" name="Coluna_F"/>
+    <tableColumn id="7" name="Coluna_G"/>
+    <tableColumn id="8" name="Coluna_H"/>
+    <tableColumn id="9" name="Coluna_I"/>
+    <tableColumn id="10" name="Coluna_J"/>
+    <tableColumn id="11" name="Coluna_K"/>
+    <tableColumn id="12" name="Coluna_L"/>
+    <tableColumn id="13" name="Coluna_M"/>
+    <tableColumn id="14" name="Coluna_N"/>
+    <tableColumn id="15" name="Coluna_O"/>
+    <tableColumn id="16" name="Coluna_P"/>
+    <tableColumn id="17" name="Coluna_Q"/>
+    <tableColumn id="18" name="Coluna_R"/>
+    <tableColumn id="19" name="Coluna_S"/>
+    <tableColumn id="20" name="Coluna_T"/>
+    <tableColumn id="21" name="Coluna_U"/>
+    <tableColumn id="22" name="Coluna_V"/>
+    <tableColumn id="23" name="Coluna_W"/>
+    <tableColumn id="24" name="Coluna_X"/>
+    <tableColumn id="25" name="Coluna_Y"/>
+    <tableColumn id="26" name="Coluna_Z"/>
+    <tableColumn id="27" name="Coluna_AA"/>
+    <tableColumn id="28" name="Coluna_AB"/>
+    <tableColumn id="29" name="Coluna_AC"/>
+    <tableColumn id="30" name="Coluna_AD"/>
+    <tableColumn id="31" name="Coluna_AE"/>
+    <tableColumn id="32" name="Coluna_AF"/>
+    <tableColumn id="33" name="Coluna_AG"/>
+    <tableColumn id="34" name="Coluna_AH"/>
+    <tableColumn id="35" name="Coluna_AI"/>
+    <tableColumn id="36" name="Coluna_AJ"/>
+    <tableColumn id="37" name="Coluna_AK"/>
+    <tableColumn id="38" name="Coluna_AL"/>
+    <tableColumn id="39" name="Coluna_AM"/>
+    <tableColumn id="40" name="Coluna_AN"/>
+    <tableColumn id="41" name="Coluna_AO"/>
+    <tableColumn id="42" name="Coluna_AP"/>
+    <tableColumn id="43" name="Coluna_AQ"/>
+    <tableColumn id="44" name="Coluna_AR"/>
+    <tableColumn id="45" name="Coluna_AS"/>
+    <tableColumn id="46" name="Coluna_AT"/>
+    <tableColumn id="47" name="Coluna_AU"/>
+    <tableColumn id="48" name="Coluna_AV"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3055,14 +3055,14 @@
   <autoFilter ref="A1:I224"/>
   <tableColumns count="9">
     <tableColumn id="1" name="CLÍNICA NEFROLÓGICA DE CARUARU LTDA."/>
-    <tableColumn id="2" name="None"/>
-    <tableColumn id="3" name="None"/>
-    <tableColumn id="4" name="None"/>
-    <tableColumn id="5" name="None"/>
-    <tableColumn id="6" name="None"/>
-    <tableColumn id="7" name="None"/>
-    <tableColumn id="8" name="None"/>
-    <tableColumn id="9" name="None"/>
+    <tableColumn id="2" name="Coluna_B"/>
+    <tableColumn id="3" name="Coluna_C"/>
+    <tableColumn id="4" name="Coluna_D"/>
+    <tableColumn id="5" name="Coluna_E"/>
+    <tableColumn id="6" name="Coluna_F"/>
+    <tableColumn id="7" name="Coluna_G"/>
+    <tableColumn id="8" name="Coluna_H"/>
+    <tableColumn id="9" name="Coluna_I"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3072,11 +3072,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="PLANILHAPAGTOSACORDOTable" displayName="PLANILHAPAGTOSACORDOTable" ref="B1:F30" headerRowCount="1">
   <autoFilter ref="B1:F30"/>
   <tableColumns count="5">
-    <tableColumn id="2" name="None"/>
-    <tableColumn id="3" name="None"/>
-    <tableColumn id="4" name="None"/>
-    <tableColumn id="5" name="None"/>
-    <tableColumn id="6" name="None"/>
+    <tableColumn id="2" name="Coluna_B"/>
+    <tableColumn id="3" name="Coluna_C"/>
+    <tableColumn id="4" name="Coluna_D"/>
+    <tableColumn id="5" name="Coluna_E"/>
+    <tableColumn id="6" name="Coluna_F"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3412,17 +3412,61 @@
           <t>CLÍNICA NEFROLÓGICA DE CARUARU LTDA.</t>
         </is>
       </c>
-      <c r="B1" s="492" t="n"/>
-      <c r="C1" s="492" t="n"/>
-      <c r="D1" s="492" t="n"/>
-      <c r="E1" s="492" t="n"/>
-      <c r="F1" s="492" t="n"/>
-      <c r="G1" s="492" t="n"/>
-      <c r="H1" s="492" t="n"/>
-      <c r="I1" s="492" t="n"/>
-      <c r="J1" s="492" t="n"/>
-      <c r="K1" s="492" t="n"/>
-      <c r="L1" s="492" t="n"/>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Coluna_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Coluna_C</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Coluna_D</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Coluna_E</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Coluna_F</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Coluna_G</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Coluna_H</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Coluna_I</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Coluna_J</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Coluna_K</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Coluna_L</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="19.8" customHeight="1">
       <c r="A2" s="476" t="inlineStr">
@@ -5773,7 +5817,7 @@
       <c r="D89" s="127" t="n"/>
       <c r="E89" s="114" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="F89" s="127" t="n"/>
@@ -10047,12 +10091,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L264"/>
-  <mergeCells count="13">
+  <mergeCells count="12">
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A235:B235"/>
     <mergeCell ref="C4:L4"/>
     <mergeCell ref="B34:C34"/>
-    <mergeCell ref="A1:L1"/>
     <mergeCell ref="C227:D227"/>
     <mergeCell ref="C226:D226"/>
     <mergeCell ref="A234:B234"/>
@@ -10174,53 +10217,241 @@
   <sheetData>
     <row r="1" ht="22" customHeight="1" thickBot="1">
       <c r="A1" s="23" t="n"/>
-      <c r="B1" s="492" t="n"/>
-      <c r="C1" s="492" t="n"/>
-      <c r="D1" s="492" t="n"/>
-      <c r="E1" s="492" t="n"/>
-      <c r="F1" s="492" t="n"/>
-      <c r="G1" s="492" t="n"/>
-      <c r="H1" s="492" t="n"/>
-      <c r="I1" s="492" t="n"/>
-      <c r="J1" s="492" t="n"/>
-      <c r="K1" s="492" t="n"/>
-      <c r="L1" s="492" t="n"/>
-      <c r="M1" s="492" t="n"/>
-      <c r="N1" s="492" t="n"/>
-      <c r="O1" s="492" t="n"/>
-      <c r="P1" s="492" t="n"/>
-      <c r="Q1" s="492" t="n"/>
-      <c r="R1" s="492" t="n"/>
-      <c r="S1" s="492" t="n"/>
-      <c r="T1" s="492" t="n"/>
-      <c r="U1" s="492" t="n"/>
-      <c r="V1" s="492" t="n"/>
-      <c r="W1" s="492" t="n"/>
-      <c r="X1" s="492" t="n"/>
-      <c r="Y1" s="492" t="n"/>
-      <c r="Z1" s="492" t="n"/>
-      <c r="AA1" s="492" t="n"/>
-      <c r="AB1" s="492" t="n"/>
-      <c r="AC1" s="492" t="n"/>
-      <c r="AD1" s="492" t="n"/>
-      <c r="AE1" s="492" t="n"/>
-      <c r="AF1" s="492" t="n"/>
-      <c r="AG1" s="492" t="n"/>
-      <c r="AH1" s="492" t="n"/>
-      <c r="AI1" s="492" t="n"/>
-      <c r="AJ1" s="492" t="n"/>
-      <c r="AK1" s="492" t="n"/>
-      <c r="AL1" s="492" t="n"/>
-      <c r="AM1" s="492" t="n"/>
-      <c r="AN1" s="492" t="n"/>
-      <c r="AO1" s="492" t="n"/>
-      <c r="AP1" s="492" t="n"/>
-      <c r="AQ1" s="492" t="n"/>
-      <c r="AR1" s="492" t="n"/>
-      <c r="AS1" s="492" t="n"/>
-      <c r="AT1" s="492" t="n"/>
-      <c r="AU1" s="492" t="n"/>
-      <c r="AV1" s="492" t="n"/>
+      <c r="B1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_B</t>
+        </is>
+      </c>
+      <c r="C1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_C</t>
+        </is>
+      </c>
+      <c r="D1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_D</t>
+        </is>
+      </c>
+      <c r="E1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_E</t>
+        </is>
+      </c>
+      <c r="F1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_F</t>
+        </is>
+      </c>
+      <c r="G1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_G</t>
+        </is>
+      </c>
+      <c r="H1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_H</t>
+        </is>
+      </c>
+      <c r="I1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_I</t>
+        </is>
+      </c>
+      <c r="J1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_J</t>
+        </is>
+      </c>
+      <c r="K1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_K</t>
+        </is>
+      </c>
+      <c r="L1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_L</t>
+        </is>
+      </c>
+      <c r="M1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_M</t>
+        </is>
+      </c>
+      <c r="N1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_N</t>
+        </is>
+      </c>
+      <c r="O1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_O</t>
+        </is>
+      </c>
+      <c r="P1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_P</t>
+        </is>
+      </c>
+      <c r="Q1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_Q</t>
+        </is>
+      </c>
+      <c r="R1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_R</t>
+        </is>
+      </c>
+      <c r="S1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_S</t>
+        </is>
+      </c>
+      <c r="T1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_T</t>
+        </is>
+      </c>
+      <c r="U1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_U</t>
+        </is>
+      </c>
+      <c r="V1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_V</t>
+        </is>
+      </c>
+      <c r="W1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_W</t>
+        </is>
+      </c>
+      <c r="X1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_X</t>
+        </is>
+      </c>
+      <c r="Y1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_Y</t>
+        </is>
+      </c>
+      <c r="Z1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_Z</t>
+        </is>
+      </c>
+      <c r="AA1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AA</t>
+        </is>
+      </c>
+      <c r="AB1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AB</t>
+        </is>
+      </c>
+      <c r="AC1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AC</t>
+        </is>
+      </c>
+      <c r="AD1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AD</t>
+        </is>
+      </c>
+      <c r="AE1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AE</t>
+        </is>
+      </c>
+      <c r="AF1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AF</t>
+        </is>
+      </c>
+      <c r="AG1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AG</t>
+        </is>
+      </c>
+      <c r="AH1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AH</t>
+        </is>
+      </c>
+      <c r="AI1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AI</t>
+        </is>
+      </c>
+      <c r="AJ1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AJ</t>
+        </is>
+      </c>
+      <c r="AK1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AK</t>
+        </is>
+      </c>
+      <c r="AL1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AL</t>
+        </is>
+      </c>
+      <c r="AM1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AM</t>
+        </is>
+      </c>
+      <c r="AN1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AN</t>
+        </is>
+      </c>
+      <c r="AO1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AO</t>
+        </is>
+      </c>
+      <c r="AP1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AP</t>
+        </is>
+      </c>
+      <c r="AQ1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AQ</t>
+        </is>
+      </c>
+      <c r="AR1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AR</t>
+        </is>
+      </c>
+      <c r="AS1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AS</t>
+        </is>
+      </c>
+      <c r="AT1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AT</t>
+        </is>
+      </c>
+      <c r="AU1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AU</t>
+        </is>
+      </c>
+      <c r="AV1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AV</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="483" t="n"/>
@@ -14097,14 +14328,46 @@
           <t>CLÍNICA NEFROLÓGICA DE CARUARU LTDA.</t>
         </is>
       </c>
-      <c r="B1" s="492" t="n"/>
-      <c r="C1" s="492" t="n"/>
-      <c r="D1" s="492" t="n"/>
-      <c r="E1" s="492" t="n"/>
-      <c r="F1" s="492" t="n"/>
-      <c r="G1" s="492" t="n"/>
-      <c r="H1" s="492" t="n"/>
-      <c r="I1" s="492" t="n"/>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Coluna_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Coluna_C</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Coluna_D</t>
+        </is>
+      </c>
+      <c r="E1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_E</t>
+        </is>
+      </c>
+      <c r="F1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_F</t>
+        </is>
+      </c>
+      <c r="G1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_G</t>
+        </is>
+      </c>
+      <c r="H1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_H</t>
+        </is>
+      </c>
+      <c r="I1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_I</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="19.8" customHeight="1">
       <c r="A2" s="489" t="inlineStr">
@@ -17559,10 +17822,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I224"/>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="A224:B224"/>
     <mergeCell ref="B205:D205"/>
-    <mergeCell ref="A1:D1"/>
     <mergeCell ref="C179:D179"/>
     <mergeCell ref="A177:B178"/>
     <mergeCell ref="A3:D3"/>
@@ -17632,11 +17894,31 @@
   <sheetData>
     <row r="1" ht="22" customHeight="1" thickBot="1">
       <c r="A1" s="23" t="n"/>
-      <c r="B1" s="492" t="n"/>
-      <c r="C1" s="492" t="n"/>
-      <c r="D1" s="492" t="n"/>
-      <c r="E1" s="492" t="n"/>
-      <c r="F1" s="492" t="n"/>
+      <c r="B1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_B</t>
+        </is>
+      </c>
+      <c r="C1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_C</t>
+        </is>
+      </c>
+      <c r="D1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_D</t>
+        </is>
+      </c>
+      <c r="E1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_E</t>
+        </is>
+      </c>
+      <c r="F1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_F</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="483" t="n"/>
@@ -18185,7 +18467,7 @@
       <c r="A27" s="28" t="n"/>
       <c r="B27" s="578" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="C27" s="409" t="inlineStr">

</xml_diff>

<commit_message>
Fix header handling in Excel table creation to support merged cells (#4)
Co-authored-by: Cursor Agent <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/Planilha SOSrim (Melhorada).xlsx
+++ b/Planilha SOSrim (Melhorada).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PLANILHA ATRAS. JAN. A JUL 2025" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PLANILHA ACORDO " sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PLANILHA PAGTOS JULHO 2025" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PLANILHA PAGTOS ACORDOS FORN." sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dashboard_Auto" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="PLANILHA ATRAS. JAN. A JUL 2025" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="PLANILHA ACORDO " sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="PLANILHA PAGTOS JULHO 2025" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="PLANILHA PAGTOS ACORDOS FORN." sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Dashboard_Auto" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PLANILHA ATRAS. JAN. A JUL 2025'!$A$1:$L$264</definedName>
@@ -2835,13 +2835,13 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -2865,7 +2865,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -2893,8 +2893,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -2920,8 +2920,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -2947,7 +2947,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>4</col>
@@ -2962,9 +2962,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -2978,17 +2978,17 @@
   <autoFilter ref="A1:L264"/>
   <tableColumns count="12">
     <tableColumn id="1" name="CLÍNICA NEFROLÓGICA DE CARUARU LTDA."/>
-    <tableColumn id="2" name="None"/>
-    <tableColumn id="3" name="None"/>
-    <tableColumn id="4" name="None"/>
-    <tableColumn id="5" name="None"/>
-    <tableColumn id="6" name="None"/>
-    <tableColumn id="7" name="None"/>
-    <tableColumn id="8" name="None"/>
-    <tableColumn id="9" name="None"/>
-    <tableColumn id="10" name="None"/>
-    <tableColumn id="11" name="None"/>
-    <tableColumn id="12" name="None"/>
+    <tableColumn id="2" name="Coluna_B"/>
+    <tableColumn id="3" name="Coluna_C"/>
+    <tableColumn id="4" name="Coluna_D"/>
+    <tableColumn id="5" name="Coluna_E"/>
+    <tableColumn id="6" name="Coluna_F"/>
+    <tableColumn id="7" name="Coluna_G"/>
+    <tableColumn id="8" name="Coluna_H"/>
+    <tableColumn id="9" name="Coluna_I"/>
+    <tableColumn id="10" name="Coluna_J"/>
+    <tableColumn id="11" name="Coluna_K"/>
+    <tableColumn id="12" name="Coluna_L"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2998,53 +2998,53 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="PLANILHAACORDOTable" displayName="PLANILHAACORDOTable" ref="B1:AV49" headerRowCount="1">
   <autoFilter ref="B1:AV49"/>
   <tableColumns count="47">
-    <tableColumn id="2" name="None"/>
-    <tableColumn id="3" name="None"/>
-    <tableColumn id="4" name="None"/>
-    <tableColumn id="5" name="None"/>
-    <tableColumn id="6" name="None"/>
-    <tableColumn id="7" name="None"/>
-    <tableColumn id="8" name="None"/>
-    <tableColumn id="9" name="None"/>
-    <tableColumn id="10" name="None"/>
-    <tableColumn id="11" name="None"/>
-    <tableColumn id="12" name="None"/>
-    <tableColumn id="13" name="None"/>
-    <tableColumn id="14" name="None"/>
-    <tableColumn id="15" name="None"/>
-    <tableColumn id="16" name="None"/>
-    <tableColumn id="17" name="None"/>
-    <tableColumn id="18" name="None"/>
-    <tableColumn id="19" name="None"/>
-    <tableColumn id="20" name="None"/>
-    <tableColumn id="21" name="None"/>
-    <tableColumn id="22" name="None"/>
-    <tableColumn id="23" name="None"/>
-    <tableColumn id="24" name="None"/>
-    <tableColumn id="25" name="None"/>
-    <tableColumn id="26" name="None"/>
-    <tableColumn id="27" name="None"/>
-    <tableColumn id="28" name="None"/>
-    <tableColumn id="29" name="None"/>
-    <tableColumn id="30" name="None"/>
-    <tableColumn id="31" name="None"/>
-    <tableColumn id="32" name="None"/>
-    <tableColumn id="33" name="None"/>
-    <tableColumn id="34" name="None"/>
-    <tableColumn id="35" name="None"/>
-    <tableColumn id="36" name="None"/>
-    <tableColumn id="37" name="None"/>
-    <tableColumn id="38" name="None"/>
-    <tableColumn id="39" name="None"/>
-    <tableColumn id="40" name="None"/>
-    <tableColumn id="41" name="None"/>
-    <tableColumn id="42" name="None"/>
-    <tableColumn id="43" name="None"/>
-    <tableColumn id="44" name="None"/>
-    <tableColumn id="45" name="None"/>
-    <tableColumn id="46" name="None"/>
-    <tableColumn id="47" name="None"/>
-    <tableColumn id="48" name="None"/>
+    <tableColumn id="2" name="Coluna_B"/>
+    <tableColumn id="3" name="Coluna_C"/>
+    <tableColumn id="4" name="Coluna_D"/>
+    <tableColumn id="5" name="Coluna_E"/>
+    <tableColumn id="6" name="Coluna_F"/>
+    <tableColumn id="7" name="Coluna_G"/>
+    <tableColumn id="8" name="Coluna_H"/>
+    <tableColumn id="9" name="Coluna_I"/>
+    <tableColumn id="10" name="Coluna_J"/>
+    <tableColumn id="11" name="Coluna_K"/>
+    <tableColumn id="12" name="Coluna_L"/>
+    <tableColumn id="13" name="Coluna_M"/>
+    <tableColumn id="14" name="Coluna_N"/>
+    <tableColumn id="15" name="Coluna_O"/>
+    <tableColumn id="16" name="Coluna_P"/>
+    <tableColumn id="17" name="Coluna_Q"/>
+    <tableColumn id="18" name="Coluna_R"/>
+    <tableColumn id="19" name="Coluna_S"/>
+    <tableColumn id="20" name="Coluna_T"/>
+    <tableColumn id="21" name="Coluna_U"/>
+    <tableColumn id="22" name="Coluna_V"/>
+    <tableColumn id="23" name="Coluna_W"/>
+    <tableColumn id="24" name="Coluna_X"/>
+    <tableColumn id="25" name="Coluna_Y"/>
+    <tableColumn id="26" name="Coluna_Z"/>
+    <tableColumn id="27" name="Coluna_AA"/>
+    <tableColumn id="28" name="Coluna_AB"/>
+    <tableColumn id="29" name="Coluna_AC"/>
+    <tableColumn id="30" name="Coluna_AD"/>
+    <tableColumn id="31" name="Coluna_AE"/>
+    <tableColumn id="32" name="Coluna_AF"/>
+    <tableColumn id="33" name="Coluna_AG"/>
+    <tableColumn id="34" name="Coluna_AH"/>
+    <tableColumn id="35" name="Coluna_AI"/>
+    <tableColumn id="36" name="Coluna_AJ"/>
+    <tableColumn id="37" name="Coluna_AK"/>
+    <tableColumn id="38" name="Coluna_AL"/>
+    <tableColumn id="39" name="Coluna_AM"/>
+    <tableColumn id="40" name="Coluna_AN"/>
+    <tableColumn id="41" name="Coluna_AO"/>
+    <tableColumn id="42" name="Coluna_AP"/>
+    <tableColumn id="43" name="Coluna_AQ"/>
+    <tableColumn id="44" name="Coluna_AR"/>
+    <tableColumn id="45" name="Coluna_AS"/>
+    <tableColumn id="46" name="Coluna_AT"/>
+    <tableColumn id="47" name="Coluna_AU"/>
+    <tableColumn id="48" name="Coluna_AV"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3055,14 +3055,14 @@
   <autoFilter ref="A1:I224"/>
   <tableColumns count="9">
     <tableColumn id="1" name="CLÍNICA NEFROLÓGICA DE CARUARU LTDA."/>
-    <tableColumn id="2" name="None"/>
-    <tableColumn id="3" name="None"/>
-    <tableColumn id="4" name="None"/>
-    <tableColumn id="5" name="None"/>
-    <tableColumn id="6" name="None"/>
-    <tableColumn id="7" name="None"/>
-    <tableColumn id="8" name="None"/>
-    <tableColumn id="9" name="None"/>
+    <tableColumn id="2" name="Coluna_B"/>
+    <tableColumn id="3" name="Coluna_C"/>
+    <tableColumn id="4" name="Coluna_D"/>
+    <tableColumn id="5" name="Coluna_E"/>
+    <tableColumn id="6" name="Coluna_F"/>
+    <tableColumn id="7" name="Coluna_G"/>
+    <tableColumn id="8" name="Coluna_H"/>
+    <tableColumn id="9" name="Coluna_I"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3072,11 +3072,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="PLANILHAPAGTOSACORDOTable" displayName="PLANILHAPAGTOSACORDOTable" ref="B1:F30" headerRowCount="1">
   <autoFilter ref="B1:F30"/>
   <tableColumns count="5">
-    <tableColumn id="2" name="None"/>
-    <tableColumn id="3" name="None"/>
-    <tableColumn id="4" name="None"/>
-    <tableColumn id="5" name="None"/>
-    <tableColumn id="6" name="None"/>
+    <tableColumn id="2" name="Coluna_B"/>
+    <tableColumn id="3" name="Coluna_C"/>
+    <tableColumn id="4" name="Coluna_D"/>
+    <tableColumn id="5" name="Coluna_E"/>
+    <tableColumn id="6" name="Coluna_F"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3412,17 +3412,61 @@
           <t>CLÍNICA NEFROLÓGICA DE CARUARU LTDA.</t>
         </is>
       </c>
-      <c r="B1" s="492" t="n"/>
-      <c r="C1" s="492" t="n"/>
-      <c r="D1" s="492" t="n"/>
-      <c r="E1" s="492" t="n"/>
-      <c r="F1" s="492" t="n"/>
-      <c r="G1" s="492" t="n"/>
-      <c r="H1" s="492" t="n"/>
-      <c r="I1" s="492" t="n"/>
-      <c r="J1" s="492" t="n"/>
-      <c r="K1" s="492" t="n"/>
-      <c r="L1" s="492" t="n"/>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Coluna_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Coluna_C</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Coluna_D</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Coluna_E</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Coluna_F</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Coluna_G</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Coluna_H</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Coluna_I</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Coluna_J</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Coluna_K</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Coluna_L</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="19.8" customHeight="1">
       <c r="A2" s="476" t="inlineStr">
@@ -5773,7 +5817,7 @@
       <c r="D89" s="127" t="n"/>
       <c r="E89" s="114" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="F89" s="127" t="n"/>
@@ -10047,12 +10091,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L264"/>
-  <mergeCells count="13">
+  <mergeCells count="12">
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A235:B235"/>
     <mergeCell ref="C4:L4"/>
     <mergeCell ref="B34:C34"/>
-    <mergeCell ref="A1:L1"/>
     <mergeCell ref="C227:D227"/>
     <mergeCell ref="C226:D226"/>
     <mergeCell ref="A234:B234"/>
@@ -10174,53 +10217,241 @@
   <sheetData>
     <row r="1" ht="22" customHeight="1" thickBot="1">
       <c r="A1" s="23" t="n"/>
-      <c r="B1" s="492" t="n"/>
-      <c r="C1" s="492" t="n"/>
-      <c r="D1" s="492" t="n"/>
-      <c r="E1" s="492" t="n"/>
-      <c r="F1" s="492" t="n"/>
-      <c r="G1" s="492" t="n"/>
-      <c r="H1" s="492" t="n"/>
-      <c r="I1" s="492" t="n"/>
-      <c r="J1" s="492" t="n"/>
-      <c r="K1" s="492" t="n"/>
-      <c r="L1" s="492" t="n"/>
-      <c r="M1" s="492" t="n"/>
-      <c r="N1" s="492" t="n"/>
-      <c r="O1" s="492" t="n"/>
-      <c r="P1" s="492" t="n"/>
-      <c r="Q1" s="492" t="n"/>
-      <c r="R1" s="492" t="n"/>
-      <c r="S1" s="492" t="n"/>
-      <c r="T1" s="492" t="n"/>
-      <c r="U1" s="492" t="n"/>
-      <c r="V1" s="492" t="n"/>
-      <c r="W1" s="492" t="n"/>
-      <c r="X1" s="492" t="n"/>
-      <c r="Y1" s="492" t="n"/>
-      <c r="Z1" s="492" t="n"/>
-      <c r="AA1" s="492" t="n"/>
-      <c r="AB1" s="492" t="n"/>
-      <c r="AC1" s="492" t="n"/>
-      <c r="AD1" s="492" t="n"/>
-      <c r="AE1" s="492" t="n"/>
-      <c r="AF1" s="492" t="n"/>
-      <c r="AG1" s="492" t="n"/>
-      <c r="AH1" s="492" t="n"/>
-      <c r="AI1" s="492" t="n"/>
-      <c r="AJ1" s="492" t="n"/>
-      <c r="AK1" s="492" t="n"/>
-      <c r="AL1" s="492" t="n"/>
-      <c r="AM1" s="492" t="n"/>
-      <c r="AN1" s="492" t="n"/>
-      <c r="AO1" s="492" t="n"/>
-      <c r="AP1" s="492" t="n"/>
-      <c r="AQ1" s="492" t="n"/>
-      <c r="AR1" s="492" t="n"/>
-      <c r="AS1" s="492" t="n"/>
-      <c r="AT1" s="492" t="n"/>
-      <c r="AU1" s="492" t="n"/>
-      <c r="AV1" s="492" t="n"/>
+      <c r="B1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_B</t>
+        </is>
+      </c>
+      <c r="C1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_C</t>
+        </is>
+      </c>
+      <c r="D1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_D</t>
+        </is>
+      </c>
+      <c r="E1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_E</t>
+        </is>
+      </c>
+      <c r="F1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_F</t>
+        </is>
+      </c>
+      <c r="G1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_G</t>
+        </is>
+      </c>
+      <c r="H1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_H</t>
+        </is>
+      </c>
+      <c r="I1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_I</t>
+        </is>
+      </c>
+      <c r="J1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_J</t>
+        </is>
+      </c>
+      <c r="K1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_K</t>
+        </is>
+      </c>
+      <c r="L1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_L</t>
+        </is>
+      </c>
+      <c r="M1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_M</t>
+        </is>
+      </c>
+      <c r="N1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_N</t>
+        </is>
+      </c>
+      <c r="O1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_O</t>
+        </is>
+      </c>
+      <c r="P1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_P</t>
+        </is>
+      </c>
+      <c r="Q1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_Q</t>
+        </is>
+      </c>
+      <c r="R1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_R</t>
+        </is>
+      </c>
+      <c r="S1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_S</t>
+        </is>
+      </c>
+      <c r="T1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_T</t>
+        </is>
+      </c>
+      <c r="U1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_U</t>
+        </is>
+      </c>
+      <c r="V1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_V</t>
+        </is>
+      </c>
+      <c r="W1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_W</t>
+        </is>
+      </c>
+      <c r="X1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_X</t>
+        </is>
+      </c>
+      <c r="Y1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_Y</t>
+        </is>
+      </c>
+      <c r="Z1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_Z</t>
+        </is>
+      </c>
+      <c r="AA1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AA</t>
+        </is>
+      </c>
+      <c r="AB1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AB</t>
+        </is>
+      </c>
+      <c r="AC1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AC</t>
+        </is>
+      </c>
+      <c r="AD1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AD</t>
+        </is>
+      </c>
+      <c r="AE1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AE</t>
+        </is>
+      </c>
+      <c r="AF1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AF</t>
+        </is>
+      </c>
+      <c r="AG1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AG</t>
+        </is>
+      </c>
+      <c r="AH1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AH</t>
+        </is>
+      </c>
+      <c r="AI1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AI</t>
+        </is>
+      </c>
+      <c r="AJ1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AJ</t>
+        </is>
+      </c>
+      <c r="AK1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AK</t>
+        </is>
+      </c>
+      <c r="AL1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AL</t>
+        </is>
+      </c>
+      <c r="AM1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AM</t>
+        </is>
+      </c>
+      <c r="AN1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AN</t>
+        </is>
+      </c>
+      <c r="AO1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AO</t>
+        </is>
+      </c>
+      <c r="AP1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AP</t>
+        </is>
+      </c>
+      <c r="AQ1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AQ</t>
+        </is>
+      </c>
+      <c r="AR1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AR</t>
+        </is>
+      </c>
+      <c r="AS1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AS</t>
+        </is>
+      </c>
+      <c r="AT1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AT</t>
+        </is>
+      </c>
+      <c r="AU1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AU</t>
+        </is>
+      </c>
+      <c r="AV1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_AV</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="483" t="n"/>
@@ -14097,14 +14328,46 @@
           <t>CLÍNICA NEFROLÓGICA DE CARUARU LTDA.</t>
         </is>
       </c>
-      <c r="B1" s="492" t="n"/>
-      <c r="C1" s="492" t="n"/>
-      <c r="D1" s="492" t="n"/>
-      <c r="E1" s="492" t="n"/>
-      <c r="F1" s="492" t="n"/>
-      <c r="G1" s="492" t="n"/>
-      <c r="H1" s="492" t="n"/>
-      <c r="I1" s="492" t="n"/>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Coluna_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Coluna_C</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Coluna_D</t>
+        </is>
+      </c>
+      <c r="E1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_E</t>
+        </is>
+      </c>
+      <c r="F1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_F</t>
+        </is>
+      </c>
+      <c r="G1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_G</t>
+        </is>
+      </c>
+      <c r="H1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_H</t>
+        </is>
+      </c>
+      <c r="I1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_I</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="19.8" customHeight="1">
       <c r="A2" s="489" t="inlineStr">
@@ -17559,10 +17822,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I224"/>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="A224:B224"/>
     <mergeCell ref="B205:D205"/>
-    <mergeCell ref="A1:D1"/>
     <mergeCell ref="C179:D179"/>
     <mergeCell ref="A177:B178"/>
     <mergeCell ref="A3:D3"/>
@@ -17632,11 +17894,31 @@
   <sheetData>
     <row r="1" ht="22" customHeight="1" thickBot="1">
       <c r="A1" s="23" t="n"/>
-      <c r="B1" s="492" t="n"/>
-      <c r="C1" s="492" t="n"/>
-      <c r="D1" s="492" t="n"/>
-      <c r="E1" s="492" t="n"/>
-      <c r="F1" s="492" t="n"/>
+      <c r="B1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_B</t>
+        </is>
+      </c>
+      <c r="C1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_C</t>
+        </is>
+      </c>
+      <c r="D1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_D</t>
+        </is>
+      </c>
+      <c r="E1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_E</t>
+        </is>
+      </c>
+      <c r="F1" s="492" t="inlineStr">
+        <is>
+          <t>Coluna_F</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="483" t="n"/>
@@ -18185,7 +18467,7 @@
       <c r="A27" s="28" t="n"/>
       <c r="B27" s="578" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="C27" s="409" t="inlineStr">

</xml_diff>